<commit_message>
Changed values (and type) for 'Number of births' from rate (fraction) to number (number)
</commit_message>
<xml_diff>
--- a/project/databook-belarus.xlsx
+++ b/project/databook-belarus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="993" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="993" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -44,39 +44,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>G</author>
-  </authors>
-  <commentList>
-    <comment ref="S10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>G:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-WB, 2000-14 crude Birth rates per 1000</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>G</author>
@@ -281,7 +248,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>G</author>
@@ -312,7 +279,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>G</author>
@@ -346,7 +313,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>G</author>
@@ -847,12 +814,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -883,26 +859,34 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -910,18 +894,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6925,13 +6926,13 @@
       <c r="D146" t="s">
         <v>12</v>
       </c>
-      <c r="N146" s="3">
+      <c r="N146" s="2">
         <v>0.23</v>
       </c>
-      <c r="O146" s="3">
+      <c r="O146" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="P146" s="3">
+      <c r="P146" s="2">
         <v>0.34</v>
       </c>
     </row>
@@ -6950,13 +6951,13 @@
       <c r="D147" t="s">
         <v>12</v>
       </c>
-      <c r="N147" s="3">
+      <c r="N147" s="2">
         <v>0.23</v>
       </c>
-      <c r="O147" s="3">
+      <c r="O147" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="P147" s="3">
+      <c r="P147" s="2">
         <v>0.34</v>
       </c>
     </row>
@@ -6975,13 +6976,13 @@
       <c r="D148" t="s">
         <v>12</v>
       </c>
-      <c r="N148" s="3">
+      <c r="N148" s="2">
         <v>0.23</v>
       </c>
-      <c r="O148" s="3">
+      <c r="O148" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="P148" s="3">
+      <c r="P148" s="2">
         <v>0.34</v>
       </c>
     </row>
@@ -7000,13 +7001,13 @@
       <c r="D149" t="s">
         <v>12</v>
       </c>
-      <c r="N149" s="3">
+      <c r="N149" s="2">
         <v>0.23</v>
       </c>
-      <c r="O149" s="3">
+      <c r="O149" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="P149" s="3">
+      <c r="P149" s="2">
         <v>0.34</v>
       </c>
     </row>
@@ -12455,7 +12456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -17916,18 +17917,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.6640625" customWidth="1"/>
     <col min="2" max="3" width="10.6640625" customWidth="1"/>
-    <col min="20" max="20" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5" customWidth="1"/>
     <col min="25" max="25" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18337,13 +18338,13 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Gen 0-4</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" ref="C10:C15" si="0">IF(SUMPRODUCT(--(E10:T10&lt;&gt;""))=0,0,"N.A.")</f>
@@ -18352,50 +18353,53 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E10">
-        <v>9.4000000000000004E-3</v>
-      </c>
-      <c r="F10">
-        <v>9.1999999999999998E-3</v>
-      </c>
-      <c r="G10">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="H10">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="I10">
-        <v>9.1000000000000004E-3</v>
-      </c>
-      <c r="J10">
-        <v>9.4000000000000004E-3</v>
-      </c>
-      <c r="K10">
-        <v>1.01E-2</v>
-      </c>
-      <c r="L10">
-        <v>1.0800000000000001E-2</v>
-      </c>
-      <c r="M10">
-        <v>1.1299999999999999E-2</v>
-      </c>
-      <c r="N10">
-        <v>1.15E-2</v>
-      </c>
-      <c r="O10">
-        <v>1.14E-2</v>
-      </c>
-      <c r="P10">
-        <v>1.15E-2</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>1.2200000000000001E-2</v>
-      </c>
-      <c r="R10">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="S10">
-        <v>1.2500000000000001E-2</v>
+      <c r="E10" s="4">
+        <v>90068.800000000003</v>
+      </c>
+      <c r="F10" s="4">
+        <v>90068.800000000003</v>
+      </c>
+      <c r="G10" s="4">
+        <v>90068.800000000003</v>
+      </c>
+      <c r="H10" s="4">
+        <v>90068.800000000003</v>
+      </c>
+      <c r="I10" s="4">
+        <v>90068.800000000003</v>
+      </c>
+      <c r="J10" s="4">
+        <v>102352.40000000001</v>
+      </c>
+      <c r="K10" s="4">
+        <v>102352.40000000001</v>
+      </c>
+      <c r="L10" s="4">
+        <v>102352.40000000001</v>
+      </c>
+      <c r="M10" s="4">
+        <v>102352.40000000001</v>
+      </c>
+      <c r="N10" s="4">
+        <v>102352.40000000001</v>
+      </c>
+      <c r="O10" s="4">
+        <v>111124.59999999999</v>
+      </c>
+      <c r="P10" s="4">
+        <v>111124.59999999999</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>111124.59999999999</v>
+      </c>
+      <c r="R10" s="4">
+        <v>111124.59999999999</v>
+      </c>
+      <c r="S10" s="4">
+        <v>111124.59999999999</v>
+      </c>
+      <c r="T10" s="4">
+        <v>109426.4</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -18404,7 +18408,7 @@
         <v>Gen 5-14</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -18420,7 +18424,7 @@
         <v>Gen 15-64</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
@@ -18436,7 +18440,7 @@
         <v>Gen 65+</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -18452,7 +18456,7 @@
         <v>PLHIV 15+</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -18468,7 +18472,7 @@
         <v>Prisoners</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
@@ -18579,22 +18583,22 @@
       <c r="M18">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18" s="2">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="O18" s="3">
+      <c r="O18" s="2">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="P18" s="3">
+      <c r="P18" s="2">
         <v>1.1999999999999999E-3</v>
       </c>
       <c r="Q18">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="R18" s="3">
+      <c r="R18" s="2">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="S18" s="3">
+      <c r="S18" s="2">
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="T18">
@@ -18789,7 +18793,7 @@
       <c r="S21">
         <v>6.6799999999999998E-2</v>
       </c>
-      <c r="T21" s="4">
+      <c r="T21" s="3">
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
@@ -18826,7 +18830,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="18">
+  <dataValidations count="13">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"Number"</formula1>
     </dataValidation>
@@ -18845,22 +18849,7 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B7">
       <formula1>"Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10">
-      <formula1>"Fraction,Number"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"Fraction,Number"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B12">
-      <formula1>"Fraction,Number"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B13">
-      <formula1>"Fraction,Number"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B14">
-      <formula1>"Fraction,Number"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10:B15">
       <formula1>"Fraction,Number"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B18">
@@ -18883,7 +18872,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Death rate (on treatment) as fractions
</commit_message>
<xml_diff>
--- a/project/databook-belarus.xlsx
+++ b/project/databook-belarus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -632,8 +632,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -644,9 +648,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1605,7 +1613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+    <sheetView topLeftCell="A130" workbookViewId="0">
       <selection activeCell="N154" sqref="N154:P157"/>
     </sheetView>
   </sheetViews>
@@ -13170,8 +13178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13592,7 +13600,7 @@
         <v>Gen 0-4</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" ref="C10:C15" si="1">IF(SUMPRODUCT(--(E10:T10&lt;&gt;""))=0,0,"N.A.")</f>
@@ -13656,7 +13664,7 @@
         <v>Gen 5-14</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -13672,7 +13680,7 @@
         <v>Gen 15-64</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
@@ -13688,7 +13696,7 @@
         <v>Gen 65+</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
@@ -13704,7 +13712,7 @@
         <v>PLHIV 15+</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
@@ -13720,7 +13728,7 @@
         <v>Prisoners</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
@@ -14078,7 +14086,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="18">
+  <dataValidations count="14">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"Number"</formula1>
     </dataValidation>
@@ -14097,22 +14105,10 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B7">
       <formula1>"Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10">
-      <formula1>"Fraction,Number"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>"Fraction,Number"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B12">
-      <formula1>"Fraction,Number"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B13">
-      <formula1>"Fraction,Number"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B14">
-      <formula1>"Fraction,Number"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B15">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10 B12 B14">
+      <formula1>"Fraction,Number"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B11 B13 B15">
       <formula1>"Fraction,Number"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B18">
@@ -14135,6 +14131,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -14147,7 +14144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T175"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>

</xml_diff>